<commit_message>
Uploaded and re-analyzed revised growth rate data with corrections to "initial" measurements. Uploaded revised figure script.
</commit_message>
<xml_diff>
--- a/Output/growth_model_coefs.xlsx
+++ b/Output/growth_model_coefs.xlsx
@@ -396,19 +396,19 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.1190079638306886</v>
+        <v>-0.07875464121263161</v>
       </c>
       <c r="C2">
-        <v>0.2228025839921209</v>
+        <v>0.2712360448979064</v>
       </c>
       <c r="D2">
-        <v>287.5789558532414</v>
+        <v>137.6354536320966</v>
       </c>
       <c r="E2">
-        <v>0.534140860031036</v>
+        <v>-0.2903546290917011</v>
       </c>
       <c r="F2">
-        <v>0.5936567398781165</v>
+        <v>0.7719819679278436</v>
       </c>
     </row>
     <row r="3">
@@ -418,19 +418,19 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.3370903342896684</v>
+        <v>0.4729630458858647</v>
       </c>
       <c r="C3">
-        <v>0.3448101175416823</v>
+        <v>0.484497005678142</v>
       </c>
       <c r="D3">
-        <v>332.6515133359218</v>
+        <v>166.3444060592113</v>
       </c>
       <c r="E3">
-        <v>-0.9776114943869629</v>
+        <v>0.976193950309077</v>
       </c>
       <c r="F3">
-        <v>0.3289769216308052</v>
+        <v>0.3303858684956607</v>
       </c>
     </row>
     <row r="4">
@@ -440,19 +440,19 @@
         </is>
       </c>
       <c r="B4">
-        <v>-0.1295099239974588</v>
+        <v>-0.3393121207190132</v>
       </c>
       <c r="C4">
-        <v>0.331672702716985</v>
+        <v>0.3960722668307303</v>
       </c>
       <c r="D4">
-        <v>356.213912833322</v>
+        <v>176.3560324640498</v>
       </c>
       <c r="E4">
-        <v>-0.3904750765937139</v>
+        <v>-0.8566924501786066</v>
       </c>
       <c r="F4">
-        <v>0.6964186868783113</v>
+        <v>0.3927774658033908</v>
       </c>
     </row>
     <row r="5">
@@ -462,19 +462,19 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.0296152209159843</v>
+        <v>0.1705593857111773</v>
       </c>
       <c r="C5">
-        <v>0.3228759458108479</v>
+        <v>0.3851890032934916</v>
       </c>
       <c r="D5">
-        <v>344.2093023481958</v>
+        <v>179.7332719118628</v>
       </c>
       <c r="E5">
-        <v>0.09172321846897179</v>
+        <v>0.4427940160618267</v>
       </c>
       <c r="F5">
-        <v>0.9269713062039875</v>
+        <v>0.6584471780563337</v>
       </c>
     </row>
     <row r="6">
@@ -484,19 +484,19 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.2854733700589905</v>
+        <v>0.6559175507094906</v>
       </c>
       <c r="C6">
-        <v>0.2770190271727857</v>
+        <v>0.3258268676812087</v>
       </c>
       <c r="D6">
-        <v>227.468904226679</v>
+        <v>126.8039750548492</v>
       </c>
       <c r="E6">
-        <v>1.030518997097378</v>
+        <v>2.013086137976949</v>
       </c>
       <c r="F6">
-        <v>0.3038609130322569</v>
+        <v>0.0462229974896117</v>
       </c>
     </row>
     <row r="7">
@@ -506,19 +506,19 @@
         </is>
       </c>
       <c r="B7">
-        <v>-0.1625067376049967</v>
+        <v>-0.6231150040980329</v>
       </c>
       <c r="C7">
-        <v>0.3655752129747366</v>
+        <v>0.567647069826566</v>
       </c>
       <c r="D7">
-        <v>542.3808190874272</v>
+        <v>273.7431405467593</v>
       </c>
       <c r="E7">
-        <v>-0.4445234026745321</v>
+        <v>-1.097715529983118</v>
       </c>
       <c r="F7">
-        <v>0.6568415319849921</v>
+        <v>0.2732933432856151</v>
       </c>
     </row>
     <row r="8">
@@ -528,19 +528,19 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.007393526639618106</v>
+        <v>-0.5955134525019619</v>
       </c>
       <c r="C8">
-        <v>0.4783768981601687</v>
+        <v>0.6478193449045511</v>
       </c>
       <c r="D8">
-        <v>350.9093567067143</v>
+        <v>181.3718460970453</v>
       </c>
       <c r="E8">
-        <v>0.015455442493259</v>
+        <v>-0.9192585204285681</v>
       </c>
       <c r="F8">
-        <v>0.9876776153912152</v>
+        <v>0.3591812996625936</v>
       </c>
     </row>
     <row r="9">
@@ -550,19 +550,19 @@
         </is>
       </c>
       <c r="B9">
-        <v>-0.514201027959193</v>
+        <v>-0.4143208248577895</v>
       </c>
       <c r="C9">
-        <v>0.4816041996446316</v>
+        <v>0.7009852699593431</v>
       </c>
       <c r="D9">
-        <v>373.8653155049074</v>
+        <v>225.109645999053</v>
       </c>
       <c r="E9">
-        <v>-1.067683853958529</v>
+        <v>-0.591054965936474</v>
       </c>
       <c r="F9">
-        <v>0.2863520691653691</v>
+        <v>0.555076586937634</v>
       </c>
     </row>
     <row r="10">
@@ -572,19 +572,19 @@
         </is>
       </c>
       <c r="B10">
-        <v>-0.2442147227219508</v>
+        <v>-0.9723398683429955</v>
       </c>
       <c r="C10">
-        <v>0.4110425716407312</v>
+        <v>0.5507690967395207</v>
       </c>
       <c r="D10">
-        <v>255.0951174897111</v>
+        <v>155.1944505260827</v>
       </c>
       <c r="E10">
-        <v>-0.5941348647833123</v>
+        <v>-1.765421978282945</v>
       </c>
       <c r="F10">
-        <v>0.5529484371950515</v>
+        <v>0.07945951067312214</v>
       </c>
     </row>
     <row r="11">
@@ -594,19 +594,19 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.04302575332546984</v>
+        <v>-0.0625419187438076</v>
       </c>
       <c r="C11">
-        <v>0.418883399759939</v>
+        <v>0.4875380440167622</v>
       </c>
       <c r="D11">
-        <v>285.2688583495349</v>
+        <v>162.8521523765324</v>
       </c>
       <c r="E11">
-        <v>0.1027153459653158</v>
+        <v>-0.1282811044416819</v>
       </c>
       <c r="F11">
-        <v>0.9182610602240131</v>
+        <v>0.8980847975208431</v>
       </c>
     </row>
     <row r="12">
@@ -616,19 +616,19 @@
         </is>
       </c>
       <c r="B12">
-        <v>-0.1692647179923663</v>
+        <v>-0.2715660407377426</v>
       </c>
       <c r="C12">
-        <v>0.4070048448179701</v>
+        <v>0.4739038328912701</v>
       </c>
       <c r="D12">
-        <v>276.3517037253818</v>
+        <v>161.3567688706566</v>
       </c>
       <c r="E12">
-        <v>-0.4158788774813446</v>
+        <v>-0.5730403974176111</v>
       </c>
       <c r="F12">
-        <v>0.6778213983410797</v>
+        <v>0.5674150503766027</v>
       </c>
     </row>
     <row r="13">
@@ -638,19 +638,19 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.6657498098762541</v>
+        <v>-0.4311303428920717</v>
       </c>
       <c r="C13">
-        <v>0.48374324061507</v>
+        <v>0.7477125507913269</v>
       </c>
       <c r="D13">
-        <v>559.2944813885996</v>
+        <v>274.4925499811952</v>
       </c>
       <c r="E13">
-        <v>1.376246227295634</v>
+        <v>-0.5765990452290701</v>
       </c>
       <c r="F13">
-        <v>0.1692961732425144</v>
+        <v>0.5646828655198403</v>
       </c>
     </row>
     <row r="14">
@@ -660,19 +660,19 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.8921921876257132</v>
+        <v>0.3709229407557811</v>
       </c>
       <c r="C14">
-        <v>0.6035906060743493</v>
+        <v>0.8064446272889852</v>
       </c>
       <c r="D14">
-        <v>556.9982291069114</v>
+        <v>272.6384218948076</v>
       </c>
       <c r="E14">
-        <v>1.478141274312368</v>
+        <v>0.4599484306848296</v>
       </c>
       <c r="F14">
-        <v>0.1399352033409275</v>
+        <v>0.6459198154282715</v>
       </c>
     </row>
     <row r="15">
@@ -682,19 +682,19 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.3225464659822507</v>
+        <v>-0.2226293547218639</v>
       </c>
       <c r="C15">
-        <v>0.4932416682991979</v>
+        <v>0.7038126702403158</v>
       </c>
       <c r="D15">
-        <v>560.9297103199444</v>
+        <v>274.9404147957764</v>
       </c>
       <c r="E15">
-        <v>0.6539319094724082</v>
+        <v>-0.3163190492803254</v>
       </c>
       <c r="F15">
-        <v>0.5134236662277556</v>
+        <v>0.7520003699713125</v>
       </c>
     </row>
     <row r="16">
@@ -704,19 +704,19 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.3872090931521088</v>
+        <v>-0.7326867164159139</v>
       </c>
       <c r="C16">
-        <v>0.4365510927563462</v>
+        <v>0.6613422261568976</v>
       </c>
       <c r="D16">
-        <v>568.1869344761805</v>
+        <v>274.9987953100372</v>
       </c>
       <c r="E16">
-        <v>-0.8869731391743948</v>
+        <v>-1.107878322957848</v>
       </c>
       <c r="F16">
-        <v>0.3754686347987368</v>
+        <v>0.2688824127433405</v>
       </c>
     </row>
     <row r="17">
@@ -726,19 +726,19 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.9257124395104481</v>
+        <v>1.46640135377371</v>
       </c>
       <c r="C17">
-        <v>0.5884458486583523</v>
+        <v>0.7552960626962272</v>
       </c>
       <c r="D17">
-        <v>279.0218407265783</v>
+        <v>165.8580198983113</v>
       </c>
       <c r="E17">
-        <v>1.573148050276943</v>
+        <v>1.941492119711318</v>
       </c>
       <c r="F17">
-        <v>0.1168177388383938</v>
+        <v>0.05389336822884208</v>
       </c>
     </row>
     <row r="18">
@@ -748,19 +748,19 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.7383630293073693</v>
+        <v>0.6567541385582069</v>
       </c>
       <c r="C18">
-        <v>0.6039508413170503</v>
+        <v>0.8091813493721264</v>
       </c>
       <c r="D18">
-        <v>303.2106965839805</v>
+        <v>204.3790638140996</v>
       </c>
       <c r="E18">
-        <v>1.222554848499264</v>
+        <v>0.8116278743545023</v>
       </c>
       <c r="F18">
-        <v>0.2224473199560815</v>
+        <v>0.4179494309640903</v>
       </c>
     </row>
     <row r="19">
@@ -770,19 +770,19 @@
         </is>
       </c>
       <c r="B19">
-        <v>-0.1963307073816335</v>
+        <v>0.3778041657856547</v>
       </c>
       <c r="C19">
-        <v>0.6494150267603152</v>
+        <v>0.9860342500620759</v>
       </c>
       <c r="D19">
-        <v>577.9469593208955</v>
+        <v>274.9913663094633</v>
       </c>
       <c r="E19">
-        <v>-0.3023193170645478</v>
+        <v>0.3831552157157523</v>
       </c>
       <c r="F19">
-        <v>0.7625174199956182</v>
+        <v>0.7019007036554604</v>
       </c>
     </row>
     <row r="20">
@@ -792,19 +792,19 @@
         </is>
       </c>
       <c r="B20">
-        <v>-0.4829630946138799</v>
+        <v>0.2917074250094386</v>
       </c>
       <c r="C20">
-        <v>0.7706834792434254</v>
+        <v>1.092927224733871</v>
       </c>
       <c r="D20">
-        <v>567.9847315303265</v>
+        <v>270.1808043850413</v>
       </c>
       <c r="E20">
-        <v>-0.626668545027073</v>
+        <v>0.26690471095225</v>
       </c>
       <c r="F20">
-        <v>0.5311283130608052</v>
+        <v>0.7897461331182813</v>
       </c>
     </row>
     <row r="21">
@@ -814,19 +814,19 @@
         </is>
       </c>
       <c r="B21">
-        <v>-0.4303326407821132</v>
+        <v>1.06799984748068</v>
       </c>
       <c r="C21">
-        <v>0.5624223078032967</v>
+        <v>0.8596073415151869</v>
       </c>
       <c r="D21">
-        <v>576.9336482922948</v>
+        <v>274.9916372831871</v>
       </c>
       <c r="E21">
-        <v>-0.76514148676446</v>
+        <v>1.242427554885897</v>
       </c>
       <c r="F21">
-        <v>0.4445001696762831</v>
+        <v>0.2151372962932173</v>
       </c>
     </row>
     <row r="22">
@@ -836,19 +836,19 @@
         </is>
       </c>
       <c r="B22">
-        <v>-0.6427425810057981</v>
+        <v>0.2053956671656148</v>
       </c>
       <c r="C22">
-        <v>0.7137603067325242</v>
+        <v>0.9405643817780359</v>
       </c>
       <c r="D22">
-        <v>571.4857792340201</v>
+        <v>274.8690356230804</v>
       </c>
       <c r="E22">
-        <v>-0.9005019961787544</v>
+        <v>0.2183749152581521</v>
       </c>
       <c r="F22">
-        <v>0.3682324725336436</v>
+        <v>0.8272990508515825</v>
       </c>
     </row>
     <row r="23">
@@ -858,19 +858,19 @@
         </is>
       </c>
       <c r="B23">
-        <v>-0.470539767556116</v>
+        <v>0.7793469430242418</v>
       </c>
       <c r="C23">
-        <v>0.6231939900525258</v>
+        <v>0.8736593374445272</v>
       </c>
       <c r="D23">
-        <v>577.5415366691616</v>
+        <v>274.1285946515516</v>
       </c>
       <c r="E23">
-        <v>-0.7550454193508135</v>
+        <v>0.8920490053982011</v>
       </c>
       <c r="F23">
-        <v>0.4505295173011721</v>
+        <v>0.3731490160142684</v>
       </c>
     </row>
     <row r="24">
@@ -880,19 +880,19 @@
         </is>
       </c>
       <c r="B24">
-        <v>-0.3063223791416003</v>
+        <v>-1.424709943635549</v>
       </c>
       <c r="C24">
-        <v>0.8008705719054262</v>
+        <v>1.178607177466117</v>
       </c>
       <c r="D24">
-        <v>583.555492016935</v>
+        <v>273.8392916307839</v>
       </c>
       <c r="E24">
-        <v>-0.3824867461577468</v>
+        <v>-1.208808134614051</v>
       </c>
       <c r="F24">
-        <v>0.7022396218281128</v>
+        <v>0.2277792798609498</v>
       </c>
     </row>
     <row r="25">
@@ -902,19 +902,19 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.1244462571589211</v>
+        <v>-1.247841531917578</v>
       </c>
       <c r="C25">
-        <v>0.9535220386192645</v>
+        <v>1.304629261775828</v>
       </c>
       <c r="D25">
-        <v>576.8924526869979</v>
+        <v>274.621892121622</v>
       </c>
       <c r="E25">
-        <v>0.1305121980600721</v>
+        <v>-0.9564721323351644</v>
       </c>
       <c r="F25">
-        <v>0.8962067004634029</v>
+        <v>0.3396749800492365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>